<commit_message>
Updated RCA jack parts
Switched out RCA jacks for gold plated parts that are also cheaper.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="166">
   <si>
     <t>Component Description</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Capacitor 0603 1uF</t>
   </si>
   <si>
-    <t>RCJ-041</t>
-  </si>
-  <si>
     <t>J1</t>
   </si>
   <si>
@@ -426,9 +423,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>these can probably be 10k. Just following the hat spec though.</t>
-  </si>
-  <si>
     <t>ERJ-3EKF1003V</t>
   </si>
   <si>
@@ -502,6 +496,24 @@
   </si>
   <si>
     <t>Light Pipe</t>
+  </si>
+  <si>
+    <t>PJRAN1X1U01AUX</t>
+  </si>
+  <si>
+    <t>Digikey</t>
+  </si>
+  <si>
+    <t>PJRAN1X1U03AU</t>
+  </si>
+  <si>
+    <t>R4 and R5 can probably be 10k. Just following the hat spec though.</t>
+  </si>
+  <si>
+    <t>SC1853-ND</t>
+  </si>
+  <si>
+    <t>SC1852-ND</t>
   </si>
 </sst>
 </file>
@@ -511,7 +523,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -532,6 +544,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -645,7 +663,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
@@ -677,6 +695,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -979,10 +998,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K37"/>
+  <dimension ref="A1:L38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -999,7 +1018,7 @@
     <col min="10" max="10" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1013,28 +1032,29 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1042,12 +1062,12 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="2"/>
+      <c r="E2" s="21"/>
       <c r="G2" s="6"/>
       <c r="H2">
         <f t="shared" ref="H2:H5" si="0">LEN(B2)-LEN(SUBSTITUTE(B2,",",""))+1</f>
@@ -1061,7 +1081,7 @@
         <v>0.24</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1069,12 +1089,12 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="21"/>
       <c r="G3" s="6"/>
       <c r="H3">
         <f t="shared" si="0"/>
@@ -1088,20 +1108,20 @@
         <v>0.38</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="21"/>
       <c r="G4" s="6"/>
       <c r="H4">
         <f t="shared" si="0"/>
@@ -1115,7 +1135,7 @@
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1123,12 +1143,12 @@
         <v>11</v>
       </c>
       <c r="C5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="21"/>
       <c r="G5" s="6"/>
       <c r="H5">
         <f t="shared" si="0"/>
@@ -1142,820 +1162,850 @@
         <v>0.34</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="21"/>
       <c r="G6" s="6"/>
       <c r="H6">
-        <f>LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
+        <f t="shared" ref="H6:H34" si="2">LEN(B6)-LEN(SUBSTITUTE(B6,",",""))+1</f>
         <v>6</v>
       </c>
       <c r="I6" s="8">
         <v>0.1</v>
       </c>
       <c r="J6" s="8">
-        <f>H6*I6</f>
+        <f t="shared" ref="J6:J35" si="3">H6*I6</f>
         <v>0.60000000000000009</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="21"/>
       <c r="G7" s="6"/>
       <c r="H7">
-        <f>LEN(B7)-LEN(SUBSTITUTE(B7,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I7" s="8">
         <v>0.1</v>
       </c>
       <c r="J7" s="8">
-        <f>H7*I7</f>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C8" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="21"/>
       <c r="G8" s="6"/>
       <c r="H8">
-        <f>LEN(B8)-LEN(SUBSTITUTE(B8,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="I8" s="8">
         <v>0.1</v>
       </c>
       <c r="J8" s="8">
-        <f>H8*I8</f>
+        <f t="shared" si="3"/>
         <v>0.5</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C9" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" s="2"/>
+        <v>58</v>
+      </c>
+      <c r="E9" s="21"/>
       <c r="G9" s="6"/>
       <c r="H9">
-        <f>LEN(B9)-LEN(SUBSTITUTE(B9,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I9" s="8">
         <v>0.1</v>
       </c>
       <c r="J9" s="8">
-        <f>H9*I9</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
-      <c r="K9" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s">
+        <v>160</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I10" s="8">
+        <v>1.04</v>
+      </c>
+      <c r="J10" s="8">
+        <f t="shared" si="3"/>
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>17</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>14</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="2" t="s">
+      <c r="C11" t="s">
+        <v>162</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E11" s="21" t="s">
+        <v>161</v>
+      </c>
+      <c r="F11" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="G10" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H10">
-        <f>LEN(B10)-LEN(SUBSTITUTE(B10,",",""))+1</f>
+      <c r="G11" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="I10" s="8">
-        <v>1.78</v>
-      </c>
-      <c r="J10" s="8">
-        <f>H10*I10</f>
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="I11" s="8">
+        <v>1.07</v>
+      </c>
+      <c r="J11" s="8">
+        <f t="shared" si="3"/>
+        <v>1.07</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>18</v>
       </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="G11" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="H11">
-        <f>LEN(B11)-LEN(SUBSTITUTE(B11,",",""))+1</f>
-        <v>1</v>
-      </c>
-      <c r="I11" s="8">
-        <v>1.78</v>
-      </c>
-      <c r="J11" s="8">
-        <f>H11*I11</f>
-        <v>1.78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>19</v>
-      </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C12" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="21"/>
       <c r="G12" s="6"/>
       <c r="H12">
-        <f>LEN(B12)-LEN(SUBSTITUTE(B12,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I12" s="8">
         <v>0.16</v>
       </c>
       <c r="J12" s="8">
-        <f>H12*I12</f>
+        <f t="shared" si="3"/>
         <v>0.32</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
         <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="2"/>
+        <v>34</v>
+      </c>
+      <c r="E13" s="21"/>
       <c r="G13" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H13">
-        <f>LEN(B13)-LEN(SUBSTITUTE(B13,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I13" s="9">
         <v>3.94</v>
       </c>
       <c r="J13" s="8">
-        <f>H13*I13</f>
+        <f t="shared" si="3"/>
         <v>3.94</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
         <v>24</v>
       </c>
-      <c r="B14" t="s">
-        <v>25</v>
-      </c>
       <c r="C14" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="E14" s="21"/>
       <c r="G14" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H14">
-        <f>LEN(B14)-LEN(SUBSTITUTE(B14,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I14" s="9">
         <v>0.62</v>
       </c>
       <c r="J14" s="8">
-        <f>H14*I14</f>
+        <f t="shared" si="3"/>
         <v>1.24</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F15" s="2">
         <v>2187</v>
       </c>
       <c r="G15" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H15">
-        <f>LEN(B15)-LEN(SUBSTITUTE(B15,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I15" s="8">
         <v>1.95</v>
       </c>
       <c r="J15" s="8">
-        <f>H15*I15</f>
+        <f t="shared" si="3"/>
         <v>1.95</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="21"/>
+      <c r="G16" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="G16" s="7" t="s">
-        <v>44</v>
-      </c>
       <c r="H16" s="11">
-        <f>LEN(B16)-LEN(SUBSTITUTE(B16,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I16" s="12">
         <v>0.56999999999999995</v>
       </c>
       <c r="J16" s="13">
-        <f>H16*I16</f>
+        <f t="shared" si="3"/>
         <v>0.56999999999999995</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>147</v>
-      </c>
+        <v>145</v>
+      </c>
+      <c r="E17" s="21"/>
       <c r="G17" s="7" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H17" s="10">
-        <f>LEN(B17)-LEN(SUBSTITUTE(B17,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I17" s="13">
         <v>0.93</v>
       </c>
       <c r="J17" s="13">
-        <f>H17*I17</f>
+        <f t="shared" si="3"/>
         <v>0.93</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
         <v>69</v>
       </c>
-      <c r="B18" t="s">
-        <v>70</v>
-      </c>
       <c r="C18" t="s">
+        <v>132</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>134</v>
-      </c>
+      <c r="E18" s="21"/>
       <c r="G18" s="17"/>
       <c r="H18" s="10">
-        <f>LEN(B18)-LEN(SUBSTITUTE(B18,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I18" s="8">
         <v>0.7</v>
       </c>
       <c r="J18" s="13">
-        <f>H18*I18</f>
+        <f t="shared" si="3"/>
         <v>0.7</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>138</v>
-      </c>
+        <v>136</v>
+      </c>
+      <c r="E19" s="21"/>
       <c r="G19" s="17"/>
       <c r="H19" s="10">
-        <f>LEN(B19)-LEN(SUBSTITUTE(B19,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I19" s="8">
         <v>0.1</v>
       </c>
       <c r="J19" s="13">
-        <f>H19*I19</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>72</v>
+      </c>
+      <c r="B20" t="s">
         <v>73</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>74</v>
       </c>
-      <c r="C20" t="s">
-        <v>75</v>
-      </c>
       <c r="D20" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E20" s="21"/>
+      <c r="G20" s="18" t="s">
         <v>131</v>
       </c>
-      <c r="G20" s="18" t="s">
-        <v>132</v>
-      </c>
       <c r="H20" s="10">
-        <f>LEN(B20)-LEN(SUBSTITUTE(B20,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I20" s="8">
         <v>0.54</v>
       </c>
       <c r="J20" s="13">
-        <f>H20*I20</f>
+        <f t="shared" si="3"/>
         <v>0.54</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>75</v>
+      </c>
+      <c r="B21" t="s">
+        <v>77</v>
+      </c>
+      <c r="C21" t="s">
         <v>76</v>
       </c>
-      <c r="B21" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" t="s">
-        <v>77</v>
-      </c>
       <c r="D21" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="E21" s="21"/>
+      <c r="G21" s="18" t="s">
         <v>129</v>
       </c>
-      <c r="G21" s="18" t="s">
-        <v>130</v>
-      </c>
       <c r="H21" s="10">
-        <f>LEN(B21)-LEN(SUBSTITUTE(B21,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I21" s="8">
         <v>1.6</v>
       </c>
       <c r="J21" s="13">
-        <f>H21*I21</f>
+        <f t="shared" si="3"/>
         <v>1.6</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B22" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C22" t="s">
+        <v>125</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="E22" s="21"/>
+      <c r="G22" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="D22" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G22" s="18" t="s">
-        <v>127</v>
-      </c>
       <c r="H22" s="10">
-        <f>LEN(B22)-LEN(SUBSTITUTE(B22,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I22" s="8">
         <v>0.77</v>
       </c>
       <c r="J22" s="13">
-        <f>H22*I22</f>
+        <f t="shared" si="3"/>
         <v>2.31</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D23" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="E23" s="21"/>
+      <c r="G23" s="18" t="s">
         <v>124</v>
       </c>
-      <c r="G23" s="18" t="s">
-        <v>125</v>
-      </c>
       <c r="H23" s="10">
-        <f>LEN(B23)-LEN(SUBSTITUTE(B23,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I23" s="8">
         <v>3.06</v>
       </c>
       <c r="J23" s="13">
-        <f>H23*I23</f>
+        <f t="shared" si="3"/>
         <v>3.06</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D24" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E24" s="21"/>
+      <c r="G24" s="18" t="s">
         <v>122</v>
       </c>
-      <c r="G24" s="18" t="s">
-        <v>123</v>
-      </c>
       <c r="H24" s="10">
-        <f>LEN(B24)-LEN(SUBSTITUTE(B24,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I24" s="8">
         <v>0.4</v>
       </c>
       <c r="J24" s="13">
-        <f>H24*I24</f>
+        <f t="shared" si="3"/>
         <v>0.4</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
+        <v>85</v>
+      </c>
+      <c r="B25" t="s">
         <v>86</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>87</v>
       </c>
-      <c r="C25" t="s">
-        <v>88</v>
-      </c>
       <c r="D25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E25" s="21"/>
+      <c r="G25" s="18" t="s">
         <v>120</v>
       </c>
-      <c r="G25" s="18" t="s">
-        <v>121</v>
-      </c>
       <c r="H25" s="10">
-        <f>LEN(B25)-LEN(SUBSTITUTE(B25,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I25" s="8">
         <v>0.49</v>
       </c>
       <c r="J25" s="13">
-        <f>H25*I25</f>
+        <f t="shared" si="3"/>
         <v>0.49</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B26" t="s">
         <v>92</v>
       </c>
-      <c r="B26" t="s">
-        <v>93</v>
-      </c>
       <c r="C26" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>140</v>
-      </c>
+        <v>138</v>
+      </c>
+      <c r="E26" s="21"/>
       <c r="G26" s="17"/>
       <c r="H26" s="10">
-        <f>LEN(B26)-LEN(SUBSTITUTE(B26,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I26" s="8">
         <v>0.1</v>
       </c>
       <c r="J26" s="13">
-        <f>H26*I26</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>93</v>
+      </c>
+      <c r="B27" t="s">
         <v>94</v>
       </c>
-      <c r="B27" t="s">
-        <v>95</v>
-      </c>
       <c r="C27" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>142</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="E27" s="21"/>
       <c r="G27" s="17"/>
       <c r="H27" s="10">
-        <f>LEN(B27)-LEN(SUBSTITUTE(B27,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="I27" s="8">
         <v>0.1</v>
       </c>
       <c r="J27" s="13">
-        <f>H27*I27</f>
+        <f t="shared" si="3"/>
         <v>0.30000000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>96</v>
+      </c>
+      <c r="B28" t="s">
         <v>97</v>
       </c>
-      <c r="B28" t="s">
-        <v>98</v>
-      </c>
       <c r="C28" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D28" s="19" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="21"/>
+      <c r="G28" s="18" t="s">
         <v>113</v>
       </c>
-      <c r="G28" s="18" t="s">
-        <v>114</v>
-      </c>
       <c r="H28" s="10">
-        <f>LEN(B28)-LEN(SUBSTITUTE(B28,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I28" s="8">
         <v>0.2</v>
       </c>
       <c r="J28" s="13">
-        <f>H28*I28</f>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>98</v>
+      </c>
+      <c r="B29" t="s">
         <v>99</v>
       </c>
-      <c r="B29" t="s">
-        <v>100</v>
-      </c>
       <c r="C29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>144</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="E29" s="21"/>
       <c r="G29" s="17"/>
       <c r="H29" s="10">
-        <f>LEN(B29)-LEN(SUBSTITUTE(B29,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I29" s="8">
         <v>0.1</v>
       </c>
       <c r="J29" s="13">
-        <f>H29*I29</f>
+        <f t="shared" si="3"/>
         <v>0.1</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C30" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>145</v>
-      </c>
+        <v>143</v>
+      </c>
+      <c r="E30" s="21"/>
       <c r="G30" s="17"/>
       <c r="H30" s="10">
-        <f>LEN(B30)-LEN(SUBSTITUTE(B30,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="I30" s="8">
         <v>0.1</v>
       </c>
       <c r="J30" s="13">
-        <f>H30*I30</f>
+        <f t="shared" si="3"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>147</v>
+      </c>
+      <c r="B31" t="s">
+        <v>156</v>
+      </c>
+      <c r="C31" t="s">
+        <v>148</v>
+      </c>
+      <c r="D31" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B31" t="s">
-        <v>158</v>
-      </c>
-      <c r="C31" t="s">
+      <c r="E31" s="21"/>
+      <c r="G31" s="18" t="s">
         <v>150</v>
       </c>
-      <c r="D31" s="2" t="s">
-        <v>151</v>
-      </c>
-      <c r="G31" s="18" t="s">
-        <v>152</v>
-      </c>
       <c r="H31" s="10">
-        <f>LEN(B31)-LEN(SUBSTITUTE(B31,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I31" s="8">
         <v>0.52</v>
       </c>
       <c r="J31" s="13">
-        <f>H31*I31</f>
+        <f t="shared" si="3"/>
         <v>0.52</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C32" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D32" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E32" s="21"/>
+      <c r="G32" s="18" t="s">
         <v>111</v>
       </c>
-      <c r="G32" s="18" t="s">
-        <v>112</v>
-      </c>
       <c r="H32" s="10">
-        <f>LEN(B32)-LEN(SUBSTITUTE(B32,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I32" s="9">
         <v>0.46</v>
       </c>
       <c r="J32" s="13">
-        <f>H32*I32</f>
+        <f t="shared" si="3"/>
         <v>0.46</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>107</v>
+      </c>
+      <c r="B33" t="s">
+        <v>157</v>
+      </c>
+      <c r="C33" t="s">
         <v>108</v>
       </c>
-      <c r="B33" t="s">
-        <v>159</v>
-      </c>
-      <c r="C33" t="s">
-        <v>109</v>
-      </c>
       <c r="D33" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="E33" s="21"/>
+      <c r="G33" s="18" t="s">
         <v>118</v>
       </c>
-      <c r="G33" s="18" t="s">
-        <v>119</v>
-      </c>
       <c r="H33" s="10">
-        <f>LEN(B33)-LEN(SUBSTITUTE(B33,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I33" s="8">
         <v>0.47</v>
       </c>
       <c r="J33" s="13">
-        <f>H33*I33</f>
+        <f t="shared" si="3"/>
         <v>0.47</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B34" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C34" t="s">
+        <v>114</v>
+      </c>
+      <c r="D34" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>116</v>
-      </c>
+      <c r="E34" s="21"/>
       <c r="G34" s="17"/>
       <c r="H34" s="11">
-        <f>LEN(B34)-LEN(SUBSTITUTE(B34,",",""))+1</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="I34" s="8">
         <v>1.71</v>
       </c>
       <c r="J34" s="13">
-        <f>H34*I34</f>
+        <f t="shared" si="3"/>
         <v>1.71</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>151</v>
+      </c>
+      <c r="B35" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C35" t="s">
         <v>153</v>
       </c>
-      <c r="B35" s="20" t="s">
+      <c r="D35" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C35" t="s">
-        <v>155</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>156</v>
-      </c>
+      <c r="E35" s="21"/>
       <c r="G35" s="17"/>
       <c r="H35" s="11">
         <v>4</v>
@@ -1964,83 +2014,87 @@
         <v>0.33</v>
       </c>
       <c r="J35" s="13">
-        <f>H35*I35</f>
+        <f t="shared" si="3"/>
         <v>1.32</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H36" s="11"/>
-      <c r="I36" s="8"/>
-      <c r="J36" s="13">
-        <f t="shared" ref="J36" si="2">H36*I36</f>
-        <v>0</v>
+      <c r="H36" s="14"/>
+      <c r="I36" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J36" s="16">
+        <f>SUM(J2:J35)</f>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H37" s="14"/>
-      <c r="I37" s="15" t="s">
-        <v>41</v>
-      </c>
-      <c r="J37" s="16">
-        <f>SUM(J3:J36)</f>
-        <v>30.209999999999997</v>
-      </c>
+      <c r="D37" s="2"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1"/>
-    <hyperlink ref="D11" r:id="rId2"/>
-    <hyperlink ref="D13" r:id="rId3"/>
-    <hyperlink ref="G11" r:id="rId4"/>
-    <hyperlink ref="G10" r:id="rId5"/>
-    <hyperlink ref="G14" r:id="rId6"/>
-    <hyperlink ref="G13" r:id="rId7"/>
-    <hyperlink ref="D16" r:id="rId8"/>
-    <hyperlink ref="G16" r:id="rId9"/>
-    <hyperlink ref="D2" r:id="rId10"/>
-    <hyperlink ref="D3" r:id="rId11"/>
-    <hyperlink ref="D4" r:id="rId12"/>
-    <hyperlink ref="D5" r:id="rId13"/>
-    <hyperlink ref="D6" r:id="rId14"/>
-    <hyperlink ref="D7" r:id="rId15"/>
-    <hyperlink ref="D8" r:id="rId16"/>
-    <hyperlink ref="D9" r:id="rId17"/>
-    <hyperlink ref="D12" r:id="rId18"/>
-    <hyperlink ref="F15" r:id="rId19" display="http://www.adafruit.com/products/2187"/>
-    <hyperlink ref="D14" r:id="rId20"/>
-    <hyperlink ref="D32" r:id="rId21"/>
-    <hyperlink ref="G32" r:id="rId22"/>
-    <hyperlink ref="D28" r:id="rId23"/>
-    <hyperlink ref="G28" r:id="rId24"/>
-    <hyperlink ref="D34" r:id="rId25"/>
-    <hyperlink ref="D33" r:id="rId26"/>
-    <hyperlink ref="G33" r:id="rId27"/>
-    <hyperlink ref="D25" r:id="rId28"/>
-    <hyperlink ref="G25" r:id="rId29"/>
-    <hyperlink ref="D24" r:id="rId30"/>
-    <hyperlink ref="G24" r:id="rId31"/>
-    <hyperlink ref="D23" r:id="rId32"/>
-    <hyperlink ref="G23" r:id="rId33"/>
-    <hyperlink ref="G22" r:id="rId34"/>
-    <hyperlink ref="D22" r:id="rId35"/>
-    <hyperlink ref="D21" r:id="rId36"/>
-    <hyperlink ref="G21" r:id="rId37"/>
-    <hyperlink ref="D20" r:id="rId38"/>
-    <hyperlink ref="G20" r:id="rId39"/>
-    <hyperlink ref="D18" r:id="rId40"/>
-    <hyperlink ref="D19" r:id="rId41"/>
-    <hyperlink ref="D26" r:id="rId42"/>
-    <hyperlink ref="D27" r:id="rId43"/>
-    <hyperlink ref="D29" r:id="rId44"/>
-    <hyperlink ref="D30" r:id="rId45"/>
-    <hyperlink ref="D17" r:id="rId46"/>
-    <hyperlink ref="G17" r:id="rId47"/>
-    <hyperlink ref="D31" r:id="rId48"/>
-    <hyperlink ref="G31" r:id="rId49"/>
-    <hyperlink ref="D35" r:id="rId50"/>
+    <hyperlink ref="D13" r:id="rId1"/>
+    <hyperlink ref="G11" r:id="rId2"/>
+    <hyperlink ref="G10" r:id="rId3"/>
+    <hyperlink ref="G14" r:id="rId4"/>
+    <hyperlink ref="G13" r:id="rId5"/>
+    <hyperlink ref="D16" r:id="rId6"/>
+    <hyperlink ref="G16" r:id="rId7"/>
+    <hyperlink ref="D2" r:id="rId8"/>
+    <hyperlink ref="D3" r:id="rId9"/>
+    <hyperlink ref="D4" r:id="rId10"/>
+    <hyperlink ref="D5" r:id="rId11"/>
+    <hyperlink ref="D6" r:id="rId12"/>
+    <hyperlink ref="D7" r:id="rId13"/>
+    <hyperlink ref="D8" r:id="rId14"/>
+    <hyperlink ref="D9" r:id="rId15"/>
+    <hyperlink ref="D12" r:id="rId16"/>
+    <hyperlink ref="F15" r:id="rId17" display="http://www.adafruit.com/products/2187"/>
+    <hyperlink ref="D14" r:id="rId18"/>
+    <hyperlink ref="D32" r:id="rId19"/>
+    <hyperlink ref="G32" r:id="rId20"/>
+    <hyperlink ref="D28" r:id="rId21"/>
+    <hyperlink ref="G28" r:id="rId22"/>
+    <hyperlink ref="D34" r:id="rId23"/>
+    <hyperlink ref="D33" r:id="rId24"/>
+    <hyperlink ref="G33" r:id="rId25"/>
+    <hyperlink ref="D25" r:id="rId26"/>
+    <hyperlink ref="G25" r:id="rId27"/>
+    <hyperlink ref="D24" r:id="rId28"/>
+    <hyperlink ref="G24" r:id="rId29"/>
+    <hyperlink ref="D23" r:id="rId30"/>
+    <hyperlink ref="G23" r:id="rId31"/>
+    <hyperlink ref="G22" r:id="rId32"/>
+    <hyperlink ref="D22" r:id="rId33"/>
+    <hyperlink ref="D21" r:id="rId34"/>
+    <hyperlink ref="G21" r:id="rId35"/>
+    <hyperlink ref="D20" r:id="rId36"/>
+    <hyperlink ref="G20" r:id="rId37"/>
+    <hyperlink ref="D18" r:id="rId38"/>
+    <hyperlink ref="D19" r:id="rId39"/>
+    <hyperlink ref="D26" r:id="rId40"/>
+    <hyperlink ref="D27" r:id="rId41"/>
+    <hyperlink ref="D29" r:id="rId42"/>
+    <hyperlink ref="D30" r:id="rId43"/>
+    <hyperlink ref="D17" r:id="rId44"/>
+    <hyperlink ref="G17" r:id="rId45"/>
+    <hyperlink ref="D31" r:id="rId46"/>
+    <hyperlink ref="G31" r:id="rId47"/>
+    <hyperlink ref="D35" r:id="rId48"/>
+    <hyperlink ref="D11" r:id="rId49"/>
+    <hyperlink ref="D10" r:id="rId50"/>
+    <hyperlink ref="F10" r:id="rId51"/>
+    <hyperlink ref="F11" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId51"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId53"/>
 </worksheet>
 </file>
 

</xml_diff>